<commit_message>
Limpieza de archivos y falta los pasis 4 y 5.
</commit_message>
<xml_diff>
--- a/Resultados_Estatus_Placa.xlsx
+++ b/Resultados_Estatus_Placa.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Estatus</t>
   </si>
@@ -23,13 +23,16 @@
     <t xml:space="preserve">Adeudos</t>
   </si>
   <si>
+    <t xml:space="preserve">Cuenta con Placa Anterior y Adeudos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuenta con Placa Anterior y Sin adeudos</t>
+  </si>
+  <si>
     <t xml:space="preserve">El número de placa no se localizó en el padrón</t>
   </si>
   <si>
     <t xml:space="preserve">EL VEHICULO FUE LOCALIZADO EN EL PADRON FISCAL DEL DISTRITO FEDERAL CON ESTATUS BAJA, ES NECESARIO QUE ACUDA A LA ADMINISTRACION TRIBUTARIA O CENTRO DE SERVICIO DE LA TESORERIA MAS CERCANO A SU DOMICILIO, A FIN DE REGISTRAR LOS DATOS DE SU VEHICULO, PRESENTANDO LOS SIGUIENTES DOCUMENTOS EN ORIGINAL Y COPIA PARA SU COTEJO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Placa anterior</t>
   </si>
   <si>
     <t xml:space="preserve">PLACA CON PROBLEMAS DE ADEUDOS DEL IMPUESTO SOBRE TENENCIA, POR LO QUE ES NECESARIO QUE EL PROPIETARIO ACUDA EXCLUSIVAMENTE A LA ADMINISTRACIÓN AUXILIAR DE CENTRO HISTÓRICO, UBICADA EN IZAZAGA 89, MEZZANINE, COL. CENTRO, A FIN DE ACLARAR SU SITUACIÓN FISCAL, PRESENTANDO LOS RECIBOS DE PAGO ORIGINALES POR LOS EJERCICIOS FISCALES DE 2005 A 2012.</t>
@@ -386,7 +389,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>346678</v>
+        <v>1150582</v>
       </c>
     </row>
     <row r="3">
@@ -394,7 +397,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>18030</v>
+        <v>303941</v>
       </c>
     </row>
     <row r="4">
@@ -402,7 +405,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>17733</v>
+        <v>155141</v>
       </c>
     </row>
     <row r="5">
@@ -410,7 +413,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>36991</v>
+        <v>72182</v>
       </c>
     </row>
     <row r="6">
@@ -418,7 +421,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>26</v>
+        <v>77384</v>
       </c>
     </row>
     <row r="7">
@@ -426,7 +429,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>206877</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8">
@@ -434,7 +437,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>237</v>
+        <v>813613</v>
       </c>
     </row>
     <row r="9">
@@ -442,7 +445,15 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>244</v>
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>